<commit_message>
Add QR scan-to-add and QR labels printing features
</commit_message>
<xml_diff>
--- a/backend/inventory_data.xlsx
+++ b/backend/inventory_data.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-12-18 19:17</t>
+          <t>2025-12-26 12:10</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M111"/>
+  <dimension ref="A1:M163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6521,6 +6521,2814 @@
       <c r="M111" t="inlineStr">
         <is>
           <t>2025-12-18 19:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>MAL20251224093200861E</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Sayı</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>1</v>
+      </c>
+      <c r="F112" t="n">
+        <v>5</v>
+      </c>
+      <c r="G112" t="n">
+        <v>3</v>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K112" t="n">
+        <v>0</v>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>MAL2025122409320057CB</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E113" t="n">
+        <v>1</v>
+      </c>
+      <c r="F113" t="n">
+        <v>5</v>
+      </c>
+      <c r="G113" t="n">
+        <v>3</v>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K113" t="n">
+        <v>0</v>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>MAL20251224093200CFCE</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E114" t="n">
+        <v>1</v>
+      </c>
+      <c r="F114" t="n">
+        <v>5</v>
+      </c>
+      <c r="G114" t="n">
+        <v>3</v>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K114" t="n">
+        <v>0</v>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>MAL202512240932002515</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>1</v>
+      </c>
+      <c r="F115" t="n">
+        <v>5</v>
+      </c>
+      <c r="G115" t="n">
+        <v>3</v>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K115" t="n">
+        <v>0</v>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>MAL20251224093200CB24</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>1</v>
+      </c>
+      <c r="F116" t="n">
+        <v>5</v>
+      </c>
+      <c r="G116" t="n">
+        <v>3</v>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K116" t="n">
+        <v>0</v>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>MAL20251224093200EA7B</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>1</v>
+      </c>
+      <c r="F117" t="n">
+        <v>5</v>
+      </c>
+      <c r="G117" t="n">
+        <v>3</v>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K117" t="n">
+        <v>0</v>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>MAL20251224093200EAE4</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E118" t="n">
+        <v>1</v>
+      </c>
+      <c r="F118" t="n">
+        <v>5</v>
+      </c>
+      <c r="G118" t="n">
+        <v>3</v>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K118" t="n">
+        <v>0</v>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>MAL2025122409320096D8</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>1</v>
+      </c>
+      <c r="F119" t="n">
+        <v>5</v>
+      </c>
+      <c r="G119" t="n">
+        <v>3</v>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K119" t="n">
+        <v>0</v>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>MAL2025122409320090EA</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>1</v>
+      </c>
+      <c r="F120" t="n">
+        <v>5</v>
+      </c>
+      <c r="G120" t="n">
+        <v>3</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K120" t="n">
+        <v>0</v>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>MAL20251224093200A305</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E121" t="n">
+        <v>1</v>
+      </c>
+      <c r="F121" t="n">
+        <v>5</v>
+      </c>
+      <c r="G121" t="n">
+        <v>3</v>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K121" t="n">
+        <v>0</v>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>MAL20251224093200B839</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E122" t="n">
+        <v>1</v>
+      </c>
+      <c r="F122" t="n">
+        <v>5</v>
+      </c>
+      <c r="G122" t="n">
+        <v>3</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K122" t="n">
+        <v>0</v>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>MAL202512240932009454</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E123" t="n">
+        <v>1</v>
+      </c>
+      <c r="F123" t="n">
+        <v>5</v>
+      </c>
+      <c r="G123" t="n">
+        <v>3</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K123" t="n">
+        <v>0</v>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>MAL20251224093200F865</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>1</v>
+      </c>
+      <c r="F124" t="n">
+        <v>5</v>
+      </c>
+      <c r="G124" t="n">
+        <v>3</v>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K124" t="n">
+        <v>0</v>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>MAL202512240932005E56</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E125" t="n">
+        <v>1</v>
+      </c>
+      <c r="F125" t="n">
+        <v>5</v>
+      </c>
+      <c r="G125" t="n">
+        <v>3</v>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K125" t="n">
+        <v>0</v>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>MAL20251224093200470E</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E126" t="n">
+        <v>1</v>
+      </c>
+      <c r="F126" t="n">
+        <v>5</v>
+      </c>
+      <c r="G126" t="n">
+        <v>3</v>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K126" t="n">
+        <v>0</v>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>MAL202512240932001997</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>1</v>
+      </c>
+      <c r="F127" t="n">
+        <v>5</v>
+      </c>
+      <c r="G127" t="n">
+        <v>3</v>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K127" t="n">
+        <v>0</v>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>MAL202512240932009550</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>1</v>
+      </c>
+      <c r="F128" t="n">
+        <v>5</v>
+      </c>
+      <c r="G128" t="n">
+        <v>3</v>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K128" t="n">
+        <v>0</v>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>MAL202512240932005757</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>1</v>
+      </c>
+      <c r="F129" t="n">
+        <v>5</v>
+      </c>
+      <c r="G129" t="n">
+        <v>3</v>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M129" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>MAL20251224093200AD03</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E130" t="n">
+        <v>1</v>
+      </c>
+      <c r="F130" t="n">
+        <v>5</v>
+      </c>
+      <c r="G130" t="n">
+        <v>3</v>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K130" t="n">
+        <v>0</v>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M130" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>MAL2025122409320056BE</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E131" t="n">
+        <v>1</v>
+      </c>
+      <c r="F131" t="n">
+        <v>5</v>
+      </c>
+      <c r="G131" t="n">
+        <v>3</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M131" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>MAL2025122409320027A8</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E132" t="n">
+        <v>1</v>
+      </c>
+      <c r="F132" t="n">
+        <v>5</v>
+      </c>
+      <c r="G132" t="n">
+        <v>3</v>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M132" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>MAL202512240932002F8F</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>1</v>
+      </c>
+      <c r="F133" t="n">
+        <v>5</v>
+      </c>
+      <c r="G133" t="n">
+        <v>3</v>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K133" t="n">
+        <v>0</v>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M133" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>MAL20251224093200E24D</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E134" t="n">
+        <v>1</v>
+      </c>
+      <c r="F134" t="n">
+        <v>5</v>
+      </c>
+      <c r="G134" t="n">
+        <v>3</v>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K134" t="n">
+        <v>0</v>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M134" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>MAL20251224093200D7C0</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E135" t="n">
+        <v>1</v>
+      </c>
+      <c r="F135" t="n">
+        <v>5</v>
+      </c>
+      <c r="G135" t="n">
+        <v>3</v>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K135" t="n">
+        <v>0</v>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>MAL20251224093200156E</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>1</v>
+      </c>
+      <c r="F136" t="n">
+        <v>5</v>
+      </c>
+      <c r="G136" t="n">
+        <v>3</v>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K136" t="n">
+        <v>0</v>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>MAL2025122409320006D4</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>1</v>
+      </c>
+      <c r="F137" t="n">
+        <v>5</v>
+      </c>
+      <c r="G137" t="n">
+        <v>3</v>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>MAL202512240932007286</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>1</v>
+      </c>
+      <c r="F138" t="n">
+        <v>5</v>
+      </c>
+      <c r="G138" t="n">
+        <v>3</v>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K138" t="n">
+        <v>0</v>
+      </c>
+      <c r="L138" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>MAL2025122409320089EF</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E139" t="n">
+        <v>1</v>
+      </c>
+      <c r="F139" t="n">
+        <v>5</v>
+      </c>
+      <c r="G139" t="n">
+        <v>3</v>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>MAL202512240932002A3E</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E140" t="n">
+        <v>1</v>
+      </c>
+      <c r="F140" t="n">
+        <v>5</v>
+      </c>
+      <c r="G140" t="n">
+        <v>3</v>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K140" t="n">
+        <v>0</v>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>MAL20251224093200D356</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E141" t="n">
+        <v>1</v>
+      </c>
+      <c r="F141" t="n">
+        <v>5</v>
+      </c>
+      <c r="G141" t="n">
+        <v>3</v>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>MAL20251224093200CCC9</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>1</v>
+      </c>
+      <c r="F142" t="n">
+        <v>5</v>
+      </c>
+      <c r="G142" t="n">
+        <v>3</v>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K142" t="n">
+        <v>0</v>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>MAL2025122409320006A1</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E143" t="n">
+        <v>1</v>
+      </c>
+      <c r="F143" t="n">
+        <v>5</v>
+      </c>
+      <c r="G143" t="n">
+        <v>3</v>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K143" t="n">
+        <v>0</v>
+      </c>
+      <c r="L143" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>MAL20251224093200FDB1</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E144" t="n">
+        <v>1</v>
+      </c>
+      <c r="F144" t="n">
+        <v>5</v>
+      </c>
+      <c r="G144" t="n">
+        <v>3</v>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K144" t="n">
+        <v>0</v>
+      </c>
+      <c r="L144" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M144" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>MAL20251224093200063E</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>1</v>
+      </c>
+      <c r="F145" t="n">
+        <v>5</v>
+      </c>
+      <c r="G145" t="n">
+        <v>3</v>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K145" t="n">
+        <v>0</v>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M145" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>MAL202512240932007781</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E146" t="n">
+        <v>1</v>
+      </c>
+      <c r="F146" t="n">
+        <v>5</v>
+      </c>
+      <c r="G146" t="n">
+        <v>3</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M146" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>MAL20251224093200EED9</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E147" t="n">
+        <v>1</v>
+      </c>
+      <c r="F147" t="n">
+        <v>5</v>
+      </c>
+      <c r="G147" t="n">
+        <v>3</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
+      <c r="L147" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M147" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>MAL202512240932003A99</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>1</v>
+      </c>
+      <c r="F148" t="n">
+        <v>5</v>
+      </c>
+      <c r="G148" t="n">
+        <v>3</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M148" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>MAL202512240932004E82</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E149" t="n">
+        <v>1</v>
+      </c>
+      <c r="F149" t="n">
+        <v>5</v>
+      </c>
+      <c r="G149" t="n">
+        <v>3</v>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K149" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M149" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>MAL2025122409320030FF</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E150" t="n">
+        <v>1</v>
+      </c>
+      <c r="F150" t="n">
+        <v>5</v>
+      </c>
+      <c r="G150" t="n">
+        <v>3</v>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K150" t="n">
+        <v>0</v>
+      </c>
+      <c r="L150" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M150" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>MAL2025122409320072D3</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>1</v>
+      </c>
+      <c r="F151" t="n">
+        <v>5</v>
+      </c>
+      <c r="G151" t="n">
+        <v>3</v>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M151" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>MAL202512240932008C47</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E152" t="n">
+        <v>1</v>
+      </c>
+      <c r="F152" t="n">
+        <v>5</v>
+      </c>
+      <c r="G152" t="n">
+        <v>3</v>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M152" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>MAL20251224093200C091</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E153" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" t="n">
+        <v>5</v>
+      </c>
+      <c r="G153" t="n">
+        <v>3</v>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K153" t="n">
+        <v>0</v>
+      </c>
+      <c r="L153" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M153" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>MAL202512240932008AF6</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>1</v>
+      </c>
+      <c r="F154" t="n">
+        <v>5</v>
+      </c>
+      <c r="G154" t="n">
+        <v>3</v>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K154" t="n">
+        <v>0</v>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>MAL20251224093200722C</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>1</v>
+      </c>
+      <c r="F155" t="n">
+        <v>5</v>
+      </c>
+      <c r="G155" t="n">
+        <v>3</v>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K155" t="n">
+        <v>0</v>
+      </c>
+      <c r="L155" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>MAL20251224093200D748</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>1</v>
+      </c>
+      <c r="F156" t="n">
+        <v>5</v>
+      </c>
+      <c r="G156" t="n">
+        <v>3</v>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K156" t="n">
+        <v>0</v>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M156" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>MAL20251224093200F55C</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E157" t="n">
+        <v>1</v>
+      </c>
+      <c r="F157" t="n">
+        <v>5</v>
+      </c>
+      <c r="G157" t="n">
+        <v>3</v>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K157" t="n">
+        <v>0</v>
+      </c>
+      <c r="L157" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>MAL20251224093200DF60</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>1</v>
+      </c>
+      <c r="F158" t="n">
+        <v>5</v>
+      </c>
+      <c r="G158" t="n">
+        <v>3</v>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K158" t="n">
+        <v>0</v>
+      </c>
+      <c r="L158" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>MAL2025122409320022F4</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>1</v>
+      </c>
+      <c r="F159" t="n">
+        <v>5</v>
+      </c>
+      <c r="G159" t="n">
+        <v>3</v>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K159" t="n">
+        <v>0</v>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>MAL202512240932008D7C</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E160" t="n">
+        <v>1</v>
+      </c>
+      <c r="F160" t="n">
+        <v>5</v>
+      </c>
+      <c r="G160" t="n">
+        <v>3</v>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K160" t="n">
+        <v>0</v>
+      </c>
+      <c r="L160" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>MAL202512240932006857</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E161" t="n">
+        <v>1</v>
+      </c>
+      <c r="F161" t="n">
+        <v>5</v>
+      </c>
+      <c r="G161" t="n">
+        <v>3</v>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K161" t="n">
+        <v>0</v>
+      </c>
+      <c r="L161" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M161" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>MAL20251224093200DF22</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E162" t="n">
+        <v>1</v>
+      </c>
+      <c r="F162" t="n">
+        <v>5</v>
+      </c>
+      <c r="G162" t="n">
+        <v>3</v>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K162" t="n">
+        <v>0</v>
+      </c>
+      <c r="L162" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>MAL202512240932007CA9</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Temizlik</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Adet</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>1</v>
+      </c>
+      <c r="F163" t="n">
+        <v>5</v>
+      </c>
+      <c r="G163" t="n">
+        <v>3</v>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Depo</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>A-1</t>
+        </is>
+      </c>
+      <c r="K163" t="n">
+        <v>0</v>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
+        </is>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>2025-12-24 09:32</t>
         </is>
       </c>
     </row>

</xml_diff>